<commit_message>
Better detection of numerical data types. Not only System.Double.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/DataTypes.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/DataTypes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <x:si>
     <x:t>Plain Text:</x:t>
   </x:si>
@@ -35,6 +35,15 @@
   </x:si>
   <x:si>
     <x:t>TimeSpan:</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Decimal Number:</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Float Number:</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Double Number:</x:t>
   </x:si>
   <x:si>
     <x:t>Explicit Text:</x:t>
@@ -529,7 +538,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C38"/>
+  <x:dimension ref="A1:C42"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -592,192 +601,216 @@
       <x:c r="B9" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="C9" s="0" t="s">
-        <x:v>1</x:v>
+      <x:c r="C9" s="0" t="n">
+        <x:v>123.45</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3">
       <x:c r="B10" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C10" s="0" t="s">
-        <x:v>9</x:v>
+      <x:c r="C10" s="0" t="n">
+        <x:v>123.45</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3">
       <x:c r="B11" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C11" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:3">
-      <x:c r="B12" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="C12" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="n">
+        <x:v>123.45</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3">
       <x:c r="B13" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3">
       <x:c r="B14" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="C14" s="4" t="s">
-        <x:v>15</x:v>
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3">
       <x:c r="B15" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C15" s="4" t="n">
-        <x:v>123.45</x:v>
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3">
       <x:c r="B16" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:3">
+      <x:c r="B17" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
         <x:v>18</x:v>
-      </x:c>
-      <x:c r="C16" s="0" t="s">
-        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:3">
       <x:c r="B18" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C18" s="4" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:3">
+      <x:c r="B19" s="0" t="s">
         <x:v>20</x:v>
+      </x:c>
+      <x:c r="C19" s="4" t="n">
+        <x:v>123.45</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:3">
       <x:c r="B20" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="C20" s="1" t="s">
+      <x:c r="C20" s="0" t="s">
         <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:3">
-      <x:c r="B21" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C21" s="2" t="s">
-        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3">
       <x:c r="B22" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="C22" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:3">
-      <x:c r="B23" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="C23" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:3">
       <x:c r="B24" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="C24" s="3" t="s">
-        <x:v>28</x:v>
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C24" s="1" t="s">
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3">
       <x:c r="B25" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="C25" s="1">
-        <x:v>40423</x:v>
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C25" s="2" t="s">
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:3">
       <x:c r="B26" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="C26" s="2">
-        <x:v>40423.5731712963</x:v>
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:3">
       <x:c r="B27" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="C27" s="0" t="b">
-        <x:v>1</x:v>
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:3">
       <x:c r="B28" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="C28" s="0" t="n">
-        <x:v>123.45</x:v>
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C28" s="3" t="s">
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:3">
       <x:c r="B29" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="C29" s="4" t="n">
-        <x:v>123.45</x:v>
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C29" s="1">
+        <x:v>40423</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:3">
       <x:c r="B30" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C30" s="2">
+        <x:v>40423.5731712963</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:3">
+      <x:c r="B31" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="C30" s="3" t="n">
-        <x:v>1.40650462962963</x:v>
+      <x:c r="C31" s="0" t="b">
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:3">
       <x:c r="B32" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="C32" s="5" t="s">
-        <x:v>22</x:v>
+      <x:c r="C32" s="0" t="n">
+        <x:v>123.45</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:3">
       <x:c r="B33" s="0" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="C33" s="6" t="s">
+      <x:c r="C33" s="4" t="n">
+        <x:v>123.45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:3">
+      <x:c r="B34" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-    </x:row>
-    <x:row r="35" spans="1:3">
-      <x:c r="B35" s="0" t="s">
+      <x:c r="C34" s="3" t="n">
+        <x:v>1.40650462962963</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:3">
+      <x:c r="B36" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="C35" s="6" t="s"/>
+      <x:c r="C36" s="5" t="s">
+        <x:v>25</x:v>
+      </x:c>
     </x:row>
     <x:row r="37" spans="1:3">
       <x:c r="B37" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="C37" s="0" t="inlineStr">
+      <x:c r="C37" s="6" t="s">
+        <x:v>40</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:3">
+      <x:c r="B39" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="C39" s="6" t="s"/>
+    </x:row>
+    <x:row r="41" spans="1:3">
+      <x:c r="B41" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="inlineStr">
         <x:is>
           <x:t>Not Shared</x:t>
         </x:is>
       </x:c>
     </x:row>
-    <x:row r="38" spans="1:3"/>
+    <x:row r="42" spans="1:3"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Don't explicitly use Convert.ToDecimal - it leads to bounds errors.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/DataTypes.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/DataTypes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <x:si>
     <x:t>Plain Text:</x:t>
   </x:si>
@@ -44,6 +44,9 @@
   </x:si>
   <x:si>
     <x:t>Double Number:</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Large Double Number:</x:t>
   </x:si>
   <x:si>
     <x:t>Explicit Text:</x:t>
@@ -538,7 +541,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C42"/>
+  <x:dimension ref="A1:C43"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -621,12 +624,12 @@
         <x:v>123.45</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:3">
-      <x:c r="B13" s="0" t="s">
+    <x:row r="12" spans="1:3">
+      <x:c r="B12" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="C13" s="0" t="s">
-        <x:v>1</x:v>
+      <x:c r="C12" s="0" t="n">
+        <x:v>9.999E+307</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3">
@@ -634,84 +637,84 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3">
       <x:c r="B15" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="C15" s="0" t="s">
-        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3">
       <x:c r="B16" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
         <x:v>15</x:v>
-      </x:c>
-      <x:c r="C16" s="0" t="s">
-        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:3">
       <x:c r="B17" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
         <x:v>17</x:v>
-      </x:c>
-      <x:c r="C17" s="0" t="s">
-        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:3">
       <x:c r="B18" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
         <x:v>19</x:v>
-      </x:c>
-      <x:c r="C18" s="4" t="s">
-        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:3">
       <x:c r="B19" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="C19" s="4" t="n">
-        <x:v>123.45</x:v>
+      <x:c r="C19" s="4" t="s">
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:3">
       <x:c r="B20" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="C20" s="0" t="s">
+      <x:c r="C20" s="4" t="n">
+        <x:v>123.45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:3">
+      <x:c r="B21" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-    </x:row>
-    <x:row r="22" spans="1:3">
-      <x:c r="B22" s="0" t="s">
+      <x:c r="C21" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
-    <x:row r="24" spans="1:3">
-      <x:c r="B24" s="0" t="s">
+    <x:row r="23" spans="1:3">
+      <x:c r="B23" s="0" t="s">
         <x:v>24</x:v>
-      </x:c>
-      <x:c r="C24" s="1" t="s">
-        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3">
       <x:c r="B25" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C25" s="1" t="s">
         <x:v>26</x:v>
-      </x:c>
-      <x:c r="C25" s="2" t="s">
-        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:3">
       <x:c r="B26" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C26" s="2" t="s">
         <x:v>28</x:v>
-      </x:c>
-      <x:c r="C26" s="0" t="s">
-        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:3">
@@ -719,54 +722,54 @@
         <x:v>29</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:3">
       <x:c r="B28" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="C28" s="3" t="s">
-        <x:v>31</x:v>
+      <x:c r="C28" s="0" t="s">
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:3">
       <x:c r="B29" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="C29" s="3" t="s">
         <x:v>32</x:v>
-      </x:c>
-      <x:c r="C29" s="1">
-        <x:v>40423</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:3">
       <x:c r="B30" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="C30" s="2">
-        <x:v>40423.5731712963</x:v>
+      <x:c r="C30" s="1">
+        <x:v>40423</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:3">
       <x:c r="B31" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="C31" s="0" t="b">
-        <x:v>1</x:v>
+      <x:c r="C31" s="2">
+        <x:v>40423.5731712963</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:3">
       <x:c r="B32" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="C32" s="0" t="n">
-        <x:v>123.45</x:v>
+      <x:c r="C32" s="0" t="b">
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:3">
       <x:c r="B33" s="0" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="C33" s="4" t="n">
+      <x:c r="C33" s="0" t="n">
         <x:v>123.45</x:v>
       </x:c>
     </x:row>
@@ -774,37 +777,45 @@
       <x:c r="B34" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="C34" s="3" t="n">
+      <x:c r="C34" s="4" t="n">
+        <x:v>123.45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:3">
+      <x:c r="B35" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C35" s="3" t="n">
         <x:v>1.40650462962963</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="36" spans="1:3">
-      <x:c r="B36" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="C36" s="5" t="s">
-        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:3">
       <x:c r="B37" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="C37" s="6" t="s">
+      <x:c r="C37" s="5" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:3">
+      <x:c r="B38" s="0" t="s">
         <x:v>40</x:v>
       </x:c>
-    </x:row>
-    <x:row r="39" spans="1:3">
-      <x:c r="B39" s="0" t="s">
+      <x:c r="C38" s="6" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="C39" s="6" t="s"/>
-    </x:row>
-    <x:row r="41" spans="1:3">
-      <x:c r="B41" s="0" t="s">
+    </x:row>
+    <x:row r="40" spans="1:3">
+      <x:c r="B40" s="0" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="C41" s="0" t="inlineStr">
+      <x:c r="C40" s="6" t="s"/>
+    </x:row>
+    <x:row r="42" spans="1:3">
+      <x:c r="B42" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="inlineStr">
         <x:is>
           <x:t>Not Shared</x:t>
         </x:is>

</xml_diff>

<commit_message>
Parse percentage too when setting datatype to numeric. Fixes #687
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/DataTypes.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/DataTypes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <x:si>
     <x:t>Plain Text:</x:t>
   </x:si>
@@ -125,6 +125,9 @@
   </x:si>
   <x:si>
     <x:t>Text to Number:</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Percentage Text to Number:</x:t>
   </x:si>
   <x:si>
     <x:t>@ format to Number:</x:t>
@@ -194,7 +197,7 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="7">
+  <x:cellStyleXfs count="8">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -210,6 +213,9 @@
     <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="10" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -217,7 +223,7 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="7">
+  <x:cellXfs count="8">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -235,6 +241,10 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -541,14 +551,14 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C43"/>
+  <x:dimension ref="A1:C44"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="25.320625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="25.920625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="21.270625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
@@ -777,24 +787,24 @@
       <x:c r="B34" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="C34" s="4" t="n">
-        <x:v>123.45</x:v>
+      <x:c r="C34" s="5" t="n">
+        <x:v>0.5512</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:3">
       <x:c r="B35" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="C35" s="3" t="n">
+      <x:c r="C35" s="4" t="n">
+        <x:v>123.45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:3">
+      <x:c r="B36" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="C36" s="3" t="n">
         <x:v>1.40650462962963</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="37" spans="1:3">
-      <x:c r="B37" s="0" t="s">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="C37" s="5" t="s">
-        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:3">
@@ -802,20 +812,28 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="C38" s="6" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:3">
+      <x:c r="B39" s="0" t="s">
         <x:v>41</x:v>
       </x:c>
-    </x:row>
-    <x:row r="40" spans="1:3">
-      <x:c r="B40" s="0" t="s">
+      <x:c r="C39" s="7" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="C40" s="6" t="s"/>
-    </x:row>
-    <x:row r="42" spans="1:3">
-      <x:c r="B42" s="0" t="s">
+    </x:row>
+    <x:row r="41" spans="1:3">
+      <x:c r="B41" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="C42" s="0" t="inlineStr">
+      <x:c r="C41" s="7" t="s"/>
+    </x:row>
+    <x:row r="43" spans="1:3">
+      <x:c r="B43" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="inlineStr">
         <x:is>
           <x:t>Not Shared</x:t>
         </x:is>

</xml_diff>